<commit_message>
getting model working on new COSIMO data (which had different formatting and countries)
</commit_message>
<xml_diff>
--- a/tables/TableS2_cosimo_genus_countries.xlsx
+++ b/tables/TableS2_cosimo_genus_countries.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cfree/Dropbox/Chris/UCSB/projects/nutrition/Health-Benefit-Calculation-BFA/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7EA998D-3FE7-4E47-92AA-CAF60EEF70C5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FA315BA-58F2-F64D-B4D8-07B3F7AD798F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="27740" yWindow="640" windowWidth="28300" windowHeight="25140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32680" yWindow="1300" windowWidth="28300" windowHeight="25140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="table" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="192">
   <si>
     <t>AFG</t>
   </si>
@@ -458,6 +458,144 @@
   </si>
   <si>
     <t>São Tomé and Príncipe</t>
+  </si>
+  <si>
+    <t>BHR</t>
+  </si>
+  <si>
+    <t>Bahrain</t>
+  </si>
+  <si>
+    <t>BTN</t>
+  </si>
+  <si>
+    <t>ERI</t>
+  </si>
+  <si>
+    <t>ESH</t>
+  </si>
+  <si>
+    <t>FSM</t>
+  </si>
+  <si>
+    <t>GNQ</t>
+  </si>
+  <si>
+    <t>MHL</t>
+  </si>
+  <si>
+    <t>PLW</t>
+  </si>
+  <si>
+    <t>PRI</t>
+  </si>
+  <si>
+    <t>QAT</t>
+  </si>
+  <si>
+    <t>SGP</t>
+  </si>
+  <si>
+    <t>SMR</t>
+  </si>
+  <si>
+    <t>TON</t>
+  </si>
+  <si>
+    <t>TUV</t>
+  </si>
+  <si>
+    <t>Bhutan</t>
+  </si>
+  <si>
+    <t>NPL</t>
+  </si>
+  <si>
+    <t>Nepal</t>
+  </si>
+  <si>
+    <t>SAU</t>
+  </si>
+  <si>
+    <t>Saudi Arabia</t>
+  </si>
+  <si>
+    <t>Eritrea</t>
+  </si>
+  <si>
+    <t>DJI</t>
+  </si>
+  <si>
+    <t>Djibouti</t>
+  </si>
+  <si>
+    <t>Western Sahara</t>
+  </si>
+  <si>
+    <t>MAR</t>
+  </si>
+  <si>
+    <t>Morocco</t>
+  </si>
+  <si>
+    <t>Micronesia (Federated States of)</t>
+  </si>
+  <si>
+    <t>Equatorial Guinea</t>
+  </si>
+  <si>
+    <t>Marshall Islands</t>
+  </si>
+  <si>
+    <t>Tonga</t>
+  </si>
+  <si>
+    <t>Tuvalu</t>
+  </si>
+  <si>
+    <t>Palau</t>
+  </si>
+  <si>
+    <t>PHL</t>
+  </si>
+  <si>
+    <t>Philippines</t>
+  </si>
+  <si>
+    <t>Puerto Rico</t>
+  </si>
+  <si>
+    <t>CUB</t>
+  </si>
+  <si>
+    <t>Cuba</t>
+  </si>
+  <si>
+    <t>Qatar</t>
+  </si>
+  <si>
+    <t>ARE</t>
+  </si>
+  <si>
+    <t>United Arab Emirates</t>
+  </si>
+  <si>
+    <t>Singapore</t>
+  </si>
+  <si>
+    <t>San Marino</t>
+  </si>
+  <si>
+    <t>MYS</t>
+  </si>
+  <si>
+    <t>Malaysia</t>
+  </si>
+  <si>
+    <t>ITA</t>
+  </si>
+  <si>
+    <t>Italy</t>
   </si>
 </sst>
 </file>
@@ -1318,16 +1456,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D42"/>
+  <dimension ref="A1:D56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -1400,206 +1538,206 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>146</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>147</v>
       </c>
       <c r="C6" t="s">
-        <v>135</v>
+        <v>164</v>
       </c>
       <c r="D6" t="s">
-        <v>136</v>
+        <v>165</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="D7" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>95</v>
+        <v>133</v>
       </c>
       <c r="D8" t="s">
-        <v>96</v>
+        <v>134</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" t="s">
-        <v>13</v>
+        <v>148</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>161</v>
       </c>
       <c r="C9" t="s">
-        <v>127</v>
+        <v>162</v>
       </c>
       <c r="D9" t="s">
-        <v>128</v>
+        <v>163</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C10" t="s">
-        <v>123</v>
+        <v>95</v>
       </c>
       <c r="D10" t="s">
-        <v>124</v>
+        <v>96</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C11" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="D11" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C12" t="s">
-        <v>101</v>
+        <v>123</v>
       </c>
       <c r="D12" t="s">
-        <v>102</v>
+        <v>124</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B13" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C13" t="s">
-        <v>95</v>
+        <v>125</v>
       </c>
       <c r="D13" t="s">
-        <v>96</v>
+        <v>126</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>22</v>
+        <v>149</v>
       </c>
       <c r="B14" t="s">
-        <v>23</v>
+        <v>166</v>
       </c>
       <c r="C14" t="s">
-        <v>87</v>
+        <v>167</v>
       </c>
       <c r="D14" t="s">
-        <v>88</v>
+        <v>168</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>24</v>
-      </c>
-      <c r="B15" t="s">
-        <v>25</v>
+        <v>150</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>169</v>
       </c>
       <c r="C15" t="s">
-        <v>89</v>
+        <v>170</v>
       </c>
       <c r="D15" t="s">
-        <v>90</v>
+        <v>171</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="B16" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="C16" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="D16" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>28</v>
+        <v>151</v>
       </c>
       <c r="B17" t="s">
-        <v>29</v>
+        <v>172</v>
       </c>
       <c r="C17" t="s">
-        <v>131</v>
+        <v>111</v>
       </c>
       <c r="D17" t="s">
-        <v>132</v>
+        <v>112</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="B18" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="C18" t="s">
-        <v>97</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>99</v>
+        <v>95</v>
+      </c>
+      <c r="D18" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>32</v>
-      </c>
-      <c r="B19" t="s">
-        <v>33</v>
+        <v>152</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>173</v>
       </c>
       <c r="C19" t="s">
-        <v>85</v>
+        <v>143</v>
       </c>
       <c r="D19" t="s">
-        <v>86</v>
+        <v>144</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="B20" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="C20" t="s">
         <v>87</v>
@@ -1610,309 +1748,505 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="B21" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="C21" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D21" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="B22" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="C22" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="D22" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="B23" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="C23" t="s">
-        <v>109</v>
+        <v>131</v>
       </c>
       <c r="D23" t="s">
-        <v>110</v>
+        <v>132</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="B24" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="C24" t="s">
-        <v>105</v>
-      </c>
-      <c r="D24" t="s">
-        <v>106</v>
+        <v>97</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="B25" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="C25" t="s">
-        <v>129</v>
+        <v>85</v>
       </c>
       <c r="D25" t="s">
-        <v>130</v>
+        <v>86</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="B26" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="C26" t="s">
-        <v>98</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>100</v>
+        <v>87</v>
+      </c>
+      <c r="D26" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>48</v>
+        <v>153</v>
       </c>
       <c r="B27" t="s">
-        <v>49</v>
+        <v>174</v>
       </c>
       <c r="C27" t="s">
-        <v>101</v>
+        <v>111</v>
       </c>
       <c r="D27" t="s">
-        <v>102</v>
+        <v>112</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="B28" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="C28" t="s">
-        <v>119</v>
+        <v>91</v>
       </c>
       <c r="D28" t="s">
-        <v>120</v>
+        <v>92</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="B29" t="s">
-        <v>145</v>
+        <v>39</v>
       </c>
       <c r="C29" t="s">
-        <v>143</v>
+        <v>107</v>
       </c>
       <c r="D29" t="s">
-        <v>144</v>
+        <v>108</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>53</v>
+        <v>154</v>
       </c>
       <c r="B30" t="s">
-        <v>54</v>
+        <v>177</v>
       </c>
       <c r="C30" t="s">
-        <v>127</v>
+        <v>178</v>
       </c>
       <c r="D30" t="s">
-        <v>128</v>
+        <v>179</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="B31" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
       <c r="C31" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="D31" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>57</v>
+        <v>155</v>
       </c>
       <c r="B32" t="s">
-        <v>58</v>
+        <v>180</v>
       </c>
       <c r="C32" t="s">
-        <v>139</v>
+        <v>181</v>
       </c>
       <c r="D32" t="s">
-        <v>140</v>
+        <v>182</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>59</v>
+        <v>42</v>
       </c>
       <c r="B33" t="s">
-        <v>60</v>
+        <v>43</v>
       </c>
       <c r="C33" t="s">
-        <v>103</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>104</v>
+        <v>105</v>
+      </c>
+      <c r="D33" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>61</v>
+        <v>156</v>
       </c>
       <c r="B34" t="s">
-        <v>62</v>
+        <v>183</v>
       </c>
       <c r="C34" t="s">
-        <v>109</v>
+        <v>184</v>
       </c>
       <c r="D34" t="s">
-        <v>110</v>
+        <v>185</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>63</v>
+        <v>157</v>
       </c>
       <c r="B35" t="s">
-        <v>64</v>
+        <v>186</v>
       </c>
       <c r="C35" t="s">
-        <v>87</v>
+        <v>188</v>
       </c>
       <c r="D35" t="s">
-        <v>88</v>
+        <v>189</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>65</v>
+        <v>44</v>
       </c>
       <c r="B36" t="s">
-        <v>66</v>
+        <v>45</v>
       </c>
       <c r="C36" t="s">
-        <v>93</v>
+        <v>129</v>
       </c>
       <c r="D36" t="s">
-        <v>94</v>
+        <v>130</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>67</v>
+        <v>46</v>
       </c>
       <c r="B37" t="s">
-        <v>68</v>
+        <v>47</v>
       </c>
       <c r="C37" t="s">
-        <v>115</v>
-      </c>
-      <c r="D37" t="s">
-        <v>116</v>
+        <v>98</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>69</v>
+        <v>158</v>
       </c>
       <c r="B38" t="s">
-        <v>70</v>
+        <v>187</v>
       </c>
       <c r="C38" t="s">
-        <v>91</v>
-      </c>
-      <c r="D38" t="s">
-        <v>92</v>
+        <v>190</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>71</v>
+        <v>48</v>
       </c>
       <c r="B39" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="C39" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="D39" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>73</v>
+        <v>50</v>
       </c>
       <c r="B40" t="s">
-        <v>74</v>
+        <v>51</v>
       </c>
       <c r="C40" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="D40" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>75</v>
+        <v>52</v>
       </c>
       <c r="B41" t="s">
-        <v>76</v>
+        <v>145</v>
       </c>
       <c r="C41" t="s">
-        <v>119</v>
+        <v>143</v>
       </c>
       <c r="D41" t="s">
-        <v>120</v>
+        <v>144</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
+        <v>53</v>
+      </c>
+      <c r="B42" t="s">
+        <v>54</v>
+      </c>
+      <c r="C42" t="s">
+        <v>127</v>
+      </c>
+      <c r="D42" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>55</v>
+      </c>
+      <c r="B43" t="s">
+        <v>56</v>
+      </c>
+      <c r="C43" t="s">
+        <v>121</v>
+      </c>
+      <c r="D43" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>57</v>
+      </c>
+      <c r="B44" t="s">
+        <v>58</v>
+      </c>
+      <c r="C44" t="s">
+        <v>139</v>
+      </c>
+      <c r="D44" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>59</v>
+      </c>
+      <c r="B45" t="s">
+        <v>60</v>
+      </c>
+      <c r="C45" t="s">
+        <v>103</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>61</v>
+      </c>
+      <c r="B46" t="s">
+        <v>62</v>
+      </c>
+      <c r="C46" t="s">
+        <v>109</v>
+      </c>
+      <c r="D46" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>159</v>
+      </c>
+      <c r="B47" t="s">
+        <v>175</v>
+      </c>
+      <c r="C47" t="s">
+        <v>111</v>
+      </c>
+      <c r="D47" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>160</v>
+      </c>
+      <c r="B48" t="s">
+        <v>176</v>
+      </c>
+      <c r="C48" t="s">
+        <v>111</v>
+      </c>
+      <c r="D48" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>63</v>
+      </c>
+      <c r="B49" t="s">
+        <v>64</v>
+      </c>
+      <c r="C49" t="s">
+        <v>87</v>
+      </c>
+      <c r="D49" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>65</v>
+      </c>
+      <c r="B50" t="s">
+        <v>66</v>
+      </c>
+      <c r="C50" t="s">
+        <v>93</v>
+      </c>
+      <c r="D50" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>67</v>
+      </c>
+      <c r="B51" t="s">
+        <v>68</v>
+      </c>
+      <c r="C51" t="s">
+        <v>115</v>
+      </c>
+      <c r="D51" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>69</v>
+      </c>
+      <c r="B52" t="s">
+        <v>70</v>
+      </c>
+      <c r="C52" t="s">
+        <v>91</v>
+      </c>
+      <c r="D52" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>71</v>
+      </c>
+      <c r="B53" t="s">
+        <v>72</v>
+      </c>
+      <c r="C53" t="s">
+        <v>111</v>
+      </c>
+      <c r="D53" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>73</v>
+      </c>
+      <c r="B54" t="s">
+        <v>74</v>
+      </c>
+      <c r="C54" t="s">
+        <v>111</v>
+      </c>
+      <c r="D54" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>75</v>
+      </c>
+      <c r="B55" t="s">
+        <v>76</v>
+      </c>
+      <c r="C55" t="s">
+        <v>119</v>
+      </c>
+      <c r="D55" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
         <v>77</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B56" t="s">
         <v>78</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C56" t="s">
         <v>117</v>
       </c>
-      <c r="D42" t="s">
+      <c r="D56" t="s">
         <v>118</v>
       </c>
     </row>

</xml_diff>

<commit_message>
worked on new intakes
</commit_message>
<xml_diff>
--- a/tables/TableS2_cosimo_genus_countries.xlsx
+++ b/tables/TableS2_cosimo_genus_countries.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cfree/Dropbox/Chris/UCSB/projects/nutrition/Health-Benefit-Calculation-BFA/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FA315BA-58F2-F64D-B4D8-07B3F7AD798F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6226B62C-2A31-1241-8453-3D62B5377F13}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32680" yWindow="1300" windowWidth="28300" windowHeight="25140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="table" sheetId="1" r:id="rId1"/>
@@ -1459,7 +1459,7 @@
   <dimension ref="A1:D56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>